<commit_message>
http api test: 添加DEBUG模式，http请求添加timout参数
</commit_message>
<xml_diff>
--- a/http_api_test/testcases/petstore_swagger.xlsx
+++ b/http_api_test/testcases/petstore_swagger.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -46,6 +46,9 @@
     <t xml:space="preserve">body</t>
   </si>
   <si>
+    <t xml:space="preserve">timeout</t>
+  </si>
+  <si>
     <t xml:space="preserve">statuscode</t>
   </si>
   <si>
@@ -59,6 +62,9 @@
   </si>
   <si>
     <t xml:space="preserve">添加一个宠物</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y</t>
   </si>
   <si>
     <t xml:space="preserve">post</t>
@@ -305,8 +311,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -318,9 +324,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="31.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="22.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="40.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="1" width="43.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="26.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="1" width="10.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="1" width="14.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="43.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="26.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="1" width="10.96"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -351,118 +358,133 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AMI1" s="1"/>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="AMJ1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="1" t="s">
         <v>18</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="166.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I5" s="7"/>
-      <c r="J5" s="1" t="s">
-        <v>33</v>
+      <c r="J5" s="7"/>
+      <c r="K5" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>